<commit_message>
sorted the table by risk-factor
</commit_message>
<xml_diff>
--- a/risk-management/risk-management.xlsx
+++ b/risk-management/risk-management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weber\Development\ptb-documentation\risk-management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88312923-0505-47E2-B9B1-BAE7EC760078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482082D5-1176-465C-AFC7-223AB524F52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F9E9B896-75D7-486D-BA38-2D6E02CB58CB}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,100 +641,103 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6">
-        <v>10</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="6">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="6">
-        <v>9</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;Crisk management</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adds values to risk factor
</commit_message>
<xml_diff>
--- a/risk-management/risk-management.xlsx
+++ b/risk-management/risk-management.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\DHBW\Software Engineering\Projekt\documentation\risk-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482082D5-1176-465C-AFC7-223AB524F52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CA87E2-B2AF-45DE-BAA4-5BA64066C696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F9E9B896-75D7-486D-BA38-2D6E02CB58CB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9E9B896-75D7-486D-BA38-2D6E02CB58CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">Risk name </t>
   </si>
@@ -93,15 +93,6 @@
     <t>predictable but uncertain</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
     <t>plan sprints in advance -&gt; distribute epics/user stories roughly on the remaining sprints; include capacity of team members in planning; keep an eye on deadlines</t>
   </si>
   <si>
@@ -130,6 +121,21 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>High (21/30)</t>
+  </si>
+  <si>
+    <t>High (18/30)</t>
+  </si>
+  <si>
+    <t>Medium (10/30)</t>
+  </si>
+  <si>
+    <t>High (12/30)</t>
+  </si>
+  <si>
+    <t>Low (3/30)</t>
   </si>
 </sst>
 </file>
@@ -558,7 +564,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,13 +615,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -632,13 +638,13 @@
         <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -655,13 +661,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -678,13 +684,13 @@
         <v>9</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -701,13 +707,13 @@
         <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -724,13 +730,13 @@
         <v>3</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds all the numbers
</commit_message>
<xml_diff>
--- a/risk-management/risk-management.xlsx
+++ b/risk-management/risk-management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\DHBW\Software Engineering\Projekt\documentation\risk-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CA87E2-B2AF-45DE-BAA4-5BA64066C696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390AB75C-3A09-4453-9BAE-8A3B707EE0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9E9B896-75D7-486D-BA38-2D6E02CB58CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t xml:space="preserve">Risk name </t>
   </si>
@@ -84,15 +84,6 @@
     <t>Fundamental issues in code base</t>
   </si>
   <si>
-    <t>known risk</t>
-  </si>
-  <si>
-    <t>unpredictable</t>
-  </si>
-  <si>
-    <t>predictable but uncertain</t>
-  </si>
-  <si>
     <t>plan sprints in advance -&gt; distribute epics/user stories roughly on the remaining sprints; include capacity of team members in planning; keep an eye on deadlines</t>
   </si>
   <si>
@@ -123,19 +114,40 @@
     <t>Tom</t>
   </si>
   <si>
-    <t>High (21/30)</t>
-  </si>
-  <si>
-    <t>High (18/30)</t>
-  </si>
-  <si>
-    <t>Medium (10/30)</t>
-  </si>
-  <si>
-    <t>High (12/30)</t>
-  </si>
-  <si>
-    <t>Low (3/30)</t>
+    <t>3 
+(known risk)</t>
+  </si>
+  <si>
+    <t>3
+(known risk)</t>
+  </si>
+  <si>
+    <t>2
+(predictable but uncertain)</t>
+  </si>
+  <si>
+    <t>1
+(unpredictable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21
+High </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12
+High </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18
+High </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10
+Medium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3
+Low </t>
   </si>
 </sst>
 </file>
@@ -218,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -245,6 +257,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,7 +579,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,8 +588,8 @@
     <col min="2" max="2" width="26.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
     <col min="7" max="7" width="18.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,34 +623,34 @@
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
+      <c r="C2" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D2" s="6">
         <v>7</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="D3" s="6">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>35</v>
@@ -644,53 +659,53 @@
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="6">
         <v>9</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -700,20 +715,20 @@
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
+      <c r="C6" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="6">
         <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -723,27 +738,27 @@
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
+      <c r="C7" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="6">
         <v>3</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;Crisk management</oddHeader>
+    <oddHeader>&amp;C&amp;"-,Fett"&amp;20Risk Management</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>